<commit_message>
TASK_6, add users table
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +634,9 @@
       <c r="D6" s="2">
         <v>41974.541666666664</v>
       </c>
+      <c r="E6" s="2">
+        <v>41975.571527777778</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -645,6 +648,9 @@
       </c>
       <c r="C7" s="2">
         <v>41974.541666666664</v>
+      </c>
+      <c r="D7" s="2">
+        <v>41975.571527777778</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -717,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
So, try back archicture
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>№</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Сделать признак аналогичности серверному.</t>
+  </si>
+  <si>
+    <t>Убрать проверку switchOff, всё равно не используется</t>
+  </si>
+  <si>
+    <t>Сделать внешние методы, либо in\out, либо setup, switchOn, switchOff</t>
+  </si>
+  <si>
+    <t>Сделать валидацию in{Name} = out{Name}</t>
   </si>
 </sst>
 </file>
@@ -519,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +676,9 @@
       <c r="C8" s="2">
         <v>41974.541666666664</v>
       </c>
+      <c r="D8" s="2">
+        <v>41975.586805555555</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -724,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,6 +887,30 @@
         <v>41974.617361111108</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3">
+        <v>41975.678472222222</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3">
+        <v>41975.691666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3">
+        <v>41975.691666666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TASK_11, completed, PageController, GUI, GUIDom, base of PageMain
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -461,21 +461,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
@@ -784,15 +814,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -803,7 +833,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" t="s">
@@ -814,293 +844,299 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>41964.652777777781</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>41964.701388888891</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>41967.652777777781</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>41964.652777777781</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>41970.701388888891</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>41973.410416666666</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>41964.652777777781</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>41968.895833333336</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>41968.9375</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>41964.652777777781</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>41969.576388888891</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <v>41969.786805555559</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>41974.504166666666</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <v>41974.541666666664</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="7">
         <v>41975.571527777778</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="9">
         <v>41974.541666666664</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="9">
         <v>41975.571527777778</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="9">
         <v>41975.586805555555</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>41974.541666666664</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <v>41975.586805555555</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>41978.646527777775</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>41974.541666666664</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="5">
         <v>41978.646527777775</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <v>41978.736805555556</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>41974.541666666664</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>41981.607638888891</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>41981.65347222222</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="6">
         <f>A10+1</f>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="7">
         <v>41974.541666666664</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="7">
         <v>41982.60833333333</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="7">
+        <v>41982.694444444445</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="8">
         <f t="shared" ref="A12:A22" si="1">A11+1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="9">
         <v>41981.541666666664</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="9">
+        <v>41982.694444444445</v>
+      </c>
+      <c r="E12" s="9">
+        <v>41982.727083333331</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>41982.541666608799</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>41983.541666608799</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="5">
         <v>41984.541666608799</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="5">
         <v>41985.541666608799</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="5">
         <v>41986.541666608799</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="5">
         <v>41987.541666608799</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="7">
         <v>41988.541666608799</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1130,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1195,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>41969.676388888889</v>
       </c>
     </row>
@@ -1167,7 +1203,7 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>41969.681944444441</v>
       </c>
     </row>
@@ -1175,7 +1211,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>41969.696527777778</v>
       </c>
     </row>
@@ -1183,7 +1219,7 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>41969.73333333333</v>
       </c>
     </row>
@@ -1191,7 +1227,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>41969.73333333333</v>
       </c>
     </row>
@@ -1199,7 +1235,7 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>41969.740972222222</v>
       </c>
     </row>
@@ -1207,7 +1243,7 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>41969.743055555555</v>
       </c>
     </row>
@@ -1215,7 +1251,7 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>41969.752083333333</v>
       </c>
     </row>
@@ -1223,7 +1259,7 @@
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>41969.754861111112</v>
       </c>
     </row>
@@ -1231,7 +1267,7 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>41973.410416666666</v>
       </c>
     </row>
@@ -1239,7 +1275,7 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>41974.5625</v>
       </c>
     </row>
@@ -1247,7 +1283,7 @@
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>41974.5625</v>
       </c>
     </row>
@@ -1258,13 +1294,13 @@
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>41974.579861111109</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>41974.579861111109</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>41974.579861111109</v>
       </c>
       <c r="F14" t="s">
@@ -1275,7 +1311,7 @@
       <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>41974.617361111108</v>
       </c>
     </row>
@@ -1283,7 +1319,7 @@
       <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>41975.678472222222</v>
       </c>
     </row>
@@ -1291,7 +1327,7 @@
       <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>41975.691666666666</v>
       </c>
     </row>
@@ -1299,7 +1335,7 @@
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>41975.691666666666</v>
       </c>
     </row>
@@ -1307,7 +1343,7 @@
       <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>41978.732638888891</v>
       </c>
     </row>
@@ -1315,7 +1351,7 @@
       <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>41982.667361111111</v>
       </c>
     </row>
@@ -1323,7 +1359,7 @@
       <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>41982.668749999997</v>
       </c>
     </row>
@@ -1331,7 +1367,7 @@
       <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>41982.668749999997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TASK_12, completed, add elementImage
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -815,7 +815,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1033,7 @@
       <c r="C12" s="9">
         <v>41981.541666666664</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>41982.694444444445</v>
       </c>
       <c r="E12" s="9">
@@ -1051,7 +1051,9 @@
       <c r="C13" s="5">
         <v>41982.541666608799</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5">
+        <v>41983.715277777781</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_13, completed add element Button
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -815,7 +815,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1054,9 @@
       <c r="D13" s="5">
         <v>41983.715277777781</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5">
+        <v>41983.770833333336</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1067,7 +1069,9 @@
       <c r="C14" s="5">
         <v>41983.541666608799</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5">
+        <v>41983.770833333336</v>
+      </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_14, completed, ElementGraphicText added
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -815,7 +815,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1072,9 @@
       <c r="D14" s="5">
         <v>41983.770833333336</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5">
+        <v>41985.643750000003</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1085,7 +1087,9 @@
       <c r="C15" s="5">
         <v>41984.541666608799</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <v>41985.664583333331</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_15, completed, created ElementFlag
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,7 +10,7 @@
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
     <sheet name="Бэклог задач" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -399,11 +399,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,7 +568,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,10 +600,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +634,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -811,14 +809,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.5703125" customWidth="1"/>
@@ -826,7 +824,7 @@
     <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -860,7 +858,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -878,7 +876,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -896,7 +894,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -914,7 +912,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -932,7 +930,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -950,7 +948,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -968,7 +966,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -986,7 +984,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1004,7 +1002,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="6">
         <f>A10+1</f>
         <v>10</v>
@@ -1022,7 +1020,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="8">
         <f t="shared" ref="A12:A22" si="1">A11+1</f>
         <v>11</v>
@@ -1040,7 +1038,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1058,7 +1056,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1076,7 +1074,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1090,9 +1088,11 @@
       <c r="D15" s="5">
         <v>41985.664583333331</v>
       </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="5">
+        <v>41985.713888888888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1103,10 +1103,14 @@
       <c r="C16" s="5">
         <v>41985.541666608799</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="5">
+        <v>41987.524305555555</v>
+      </c>
+      <c r="E16" s="5">
+        <v>41987.615972222222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1120,7 +1124,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1134,7 +1138,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1148,19 +1152,19 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1173,21 +1177,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="72.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>10</v>
       </c>
@@ -1201,7 +1205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +1213,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1217,7 +1221,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1237,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1241,7 +1245,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -1257,7 +1261,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1265,7 +1269,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1277,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1281,7 +1285,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1289,7 +1293,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1297,7 +1301,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1317,7 +1321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1333,7 +1337,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1345,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -1349,7 +1353,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -1357,7 +1361,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
         <v>47</v>
       </c>
@@ -1365,7 +1369,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>48</v>
       </c>
@@ -1373,7 +1377,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
TASK_16, completed, create ElementRadio
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -813,7 +813,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1121,8 +1121,12 @@
       <c r="C17" s="5">
         <v>41986.541666608799</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="5">
+        <v>41987.674305555556</v>
+      </c>
+      <c r="E17" s="5">
+        <v>41987.707638888889</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3">

</xml_diff>

<commit_message>
TASK_17, completed add score indicator
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>№</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>сделать клиент-серверный независимый MD5(для соцсети)</t>
+  </si>
+  <si>
+    <t>3.9 - Элемент Игровое поле.(ElementField)</t>
   </si>
 </sst>
 </file>
@@ -403,12 +406,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,7 +499,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -499,10 +510,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -810,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1022,7 +1033,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="8">
-        <f t="shared" ref="A12:A22" si="1">A11+1</f>
+        <f t="shared" ref="A12:A24" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1047,7 +1058,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="5">
-        <v>41982.541666608799</v>
+        <v>41981.541666666664</v>
       </c>
       <c r="D13" s="5">
         <v>41983.715277777781</v>
@@ -1065,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="5">
-        <v>41983.541666608799</v>
+        <v>41981.541666666664</v>
       </c>
       <c r="D14" s="5">
         <v>41983.770833333336</v>
@@ -1083,7 +1094,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="5">
-        <v>41984.541666608799</v>
+        <v>41981.541666666664</v>
       </c>
       <c r="D15" s="5">
         <v>41985.664583333331</v>
@@ -1101,7 +1112,7 @@
         <v>43</v>
       </c>
       <c r="C16" s="5">
-        <v>41985.541666608799</v>
+        <v>41981.541666666664</v>
       </c>
       <c r="D16" s="5">
         <v>41987.524305555555</v>
@@ -1119,7 +1130,7 @@
         <v>44</v>
       </c>
       <c r="C17" s="5">
-        <v>41986.541666608799</v>
+        <v>41981.541666666664</v>
       </c>
       <c r="D17" s="5">
         <v>41987.674305555556</v>
@@ -1137,41 +1148,65 @@
         <v>45</v>
       </c>
       <c r="C18" s="5">
-        <v>41987.541666608799</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+        <v>41981.541666666664</v>
+      </c>
+      <c r="D18" s="5">
+        <v>41987.758333333331</v>
+      </c>
+      <c r="E18" s="5">
+        <v>41987.765277777777</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="6">
+      <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="7">
-        <v>41988.541666608799</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="5">
+        <v>41981.541666666664</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20">
+      <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
+      <c r="B20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="7">
+        <v>41987.755555555559</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21">
+      <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="A22" s="3">
         <f t="shared" si="1"/>
         <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3">
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TASK_19, completed, add ElementField
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
     <sheet name="Бэклог задач" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>№</t>
   </si>
@@ -397,16 +397,19 @@
   </si>
   <si>
     <t>3.9 - Элемент Игровое поле.(ElementField)</t>
+  </si>
+  <si>
+    <t>сделать страницы, блоки и включить блоки в страницы.(бэкграунд,чат)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,7 +582,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,9 +614,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,6 +649,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -820,14 +825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.5703125" customWidth="1"/>
@@ -835,7 +840,7 @@
     <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -852,7 +857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -869,7 +874,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -887,7 +892,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -905,7 +910,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -923,7 +928,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -941,7 +946,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -959,7 +964,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -977,7 +982,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -995,7 +1000,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1013,7 +1018,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f>A10+1</f>
         <v>10</v>
@@ -1031,7 +1036,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f t="shared" ref="A12:A24" si="1">A11+1</f>
         <v>11</v>
@@ -1049,7 +1054,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1067,7 +1072,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1085,7 +1090,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1103,7 +1108,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1121,7 +1126,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1139,7 +1144,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1157,7 +1162,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1171,7 +1176,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1182,28 +1187,30 @@
       <c r="C20" s="7">
         <v>41987.755555555559</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="5">
+        <v>41987.771527777775</v>
+      </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1216,21 +1223,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="72.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>10</v>
       </c>
@@ -1244,7 +1251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1259,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1267,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1268,7 +1275,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -1276,7 +1283,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1284,7 +1291,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -1300,7 +1307,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1308,7 +1315,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -1316,7 +1323,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1324,7 +1331,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1332,7 +1339,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1340,7 +1347,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1360,7 +1367,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -1368,7 +1375,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -1400,7 +1407,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>47</v>
       </c>
@@ -1408,7 +1415,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>48</v>
       </c>
@@ -1416,12 +1423,20 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="2">
         <v>41982.668749999997</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2">
+        <v>41988.625694444447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TASK_18, completed main and game pages.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>№</t>
   </si>
@@ -400,6 +400,149 @@
   </si>
   <si>
     <t>сделать страницы, блоки и включить блоки в страницы.(бэкграунд,чат)</t>
+  </si>
+  <si>
+    <t>4.1 – Таблица игр. (DB.games)</t>
+  </si>
+  <si>
+    <r>
+      <t>4.2 – Функционал создания игры. (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogicGame.createGame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.3 - Покинуть игру. (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogicGame.closeGame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.4 – Ход игроком. (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogicGame.doMove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.5 – Проверка победителя. (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogicGame.checkWinner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.6 – Начисление очков. (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogicUser.onWin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -409,12 +552,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -497,12 +648,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -513,10 +664,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -826,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1198,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ref="A12:A24" si="1">A11+1</f>
+        <f t="shared" ref="A12:A26" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1173,11 +1333,15 @@
       <c r="C19" s="5">
         <v>41981.541666666664</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="5">
+        <v>41988.74722222222</v>
+      </c>
+      <c r="E19" s="5">
+        <v>41989.681944444441</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -1187,34 +1351,86 @@
       <c r="C20" s="7">
         <v>41987.755555555559</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="7">
         <v>41987.771527777775</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7">
+        <v>41988.74722222222</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
+      <c r="B21" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="9">
+        <v>41989.640972222223</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
+      <c r="B22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="5">
+        <v>41989.640972222223</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
+      <c r="B23" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="5">
+        <v>41989.640972222223</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
+      <c r="B24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="5">
+        <v>41989.640972222223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="5">
+        <v>41989.640972222223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="7">
+        <v>41989.640972222223</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1226,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TASK_20, completed, create table games
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -989,7 +989,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,6 +1368,12 @@
       </c>
       <c r="C21" s="9">
         <v>41989.640972222223</v>
+      </c>
+      <c r="D21" s="9">
+        <v>41989.693749999999</v>
+      </c>
+      <c r="E21" s="9">
+        <v>41989.708333333336</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_21 comleted, createGame realized
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -552,12 +552,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -648,12 +656,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -664,22 +672,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
@@ -989,7 +1000,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,6 +1398,12 @@
       <c r="C22" s="5">
         <v>41989.640972222223</v>
       </c>
+      <c r="D22" s="5">
+        <v>41989.726388888892</v>
+      </c>
+      <c r="E22" s="5">
+        <v>41996.762499999997</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1405,7 +1422,7 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="17" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="5">

</xml_diff>

<commit_message>
TASK_22, completed! close game mechanizm realized.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,6 +1415,9 @@
       </c>
       <c r="C23" s="5">
         <v>41989.640972222223</v>
+      </c>
+      <c r="D23" s="5">
+        <v>41996.777083333334</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_23, - completed, doMove realized
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,6 +1419,9 @@
       <c r="D23" s="5">
         <v>41996.777083333334</v>
       </c>
+      <c r="E23" s="5">
+        <v>41996.859027777777</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1430,6 +1433,12 @@
       </c>
       <c r="C24" s="5">
         <v>41989.640972222223</v>
+      </c>
+      <c r="D24" s="5">
+        <v>41997.734027777777</v>
+      </c>
+      <c r="E24" s="5">
+        <v>41998.57708333333</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_26, comleted, ElementChatWindow realized
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>№</t>
   </si>
@@ -543,6 +543,21 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>7.2 - Элемент ввода сообщения. (ElementChatInput)</t>
+  </si>
+  <si>
+    <t>7.1. - Элемент окно чата. (ElemenChatWindow)</t>
+  </si>
+  <si>
+    <t>7.3 - Функционал отправки сообщений. (LogicChat.sendMessage)</t>
+  </si>
+  <si>
+    <t>7.4 - Расслыка сообщений игрокам. (LogicChat.sendMessageAll)</t>
+  </si>
+  <si>
+    <t>7.5 - Запрос последних сообщений. (LogicChat.getLastMessages)</t>
   </si>
 </sst>
 </file>
@@ -552,12 +567,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -656,12 +679,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -672,25 +695,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
@@ -997,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,7 +1238,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ref="A12:A26" si="1">A11+1</f>
+        <f t="shared" ref="A12:A31" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1476,6 +1505,77 @@
       <c r="E26" s="7">
         <v>41999.656944444447</v>
       </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="5">
+        <v>42000.640972222223</v>
+      </c>
+      <c r="D27" s="5">
+        <v>42000.640972222223</v>
+      </c>
+      <c r="E27" s="5">
+        <v>42002.667361111111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="5">
+        <v>42000.640972222223</v>
+      </c>
+      <c r="D28" s="5">
+        <v>42002.667361111111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="5">
+        <v>42000.640972222223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="5">
+        <v>42000.640972222223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="7">
+        <v>42000.640972222223</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TASK_31, update friends type completed.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -594,8 +594,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy\ h:mm"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -725,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -771,6 +772,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1097,7 +1099,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1611,36 +1613,36 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="26">
+      <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="25">
         <v>42000.640972222223</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="25">
         <v>42006.01666666667</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="25">
         <v>42006.890277777777</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="26"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="27"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3">
@@ -1671,7 +1673,7 @@
       <c r="C33" s="5">
         <v>42008.844444444447</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="21">
         <v>42010.817361111112</v>
       </c>
       <c r="E33" s="2">
@@ -1688,6 +1690,12 @@
       </c>
       <c r="C34" s="5">
         <v>42008.844444444447</v>
+      </c>
+      <c r="D34" s="21">
+        <v>42011.99722222222</v>
+      </c>
+      <c r="E34" s="2">
+        <v>42013.111111111109</v>
       </c>
     </row>
     <row r="35" spans="1:5">

</xml_diff>

<commit_message>
TASK_32, completed, Robot create game
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>№</t>
   </si>
@@ -588,15 +588,29 @@
     <t xml:space="preserve">7.3 - Функционал отправки сообщений. (LogicChat.sendMessage)
 7.5 - Запрос последних сообщений. (LogicChat.getLastMessages)
 7.4 - Расслыка сообщений игрокам. (LogicChat.sendMessageAll) </t>
+  </si>
+  <si>
+    <t>5.1 – Создание игры с роботом. (LogicRobot.createGame)</t>
+  </si>
+  <si>
+    <t>5.2 – Ход роботом. (LogicRobot.AIDoMove#1)</t>
+  </si>
+  <si>
+    <t>5.3 – Мозг робота. (LogicRobot.AIDoMove#2)</t>
+  </si>
+  <si>
+    <t>5.4 – Проверка победителя. (LogicRobot.checkWinner)</t>
+  </si>
+  <si>
+    <t>5.5 – Покинуть и игру с роботом. (LogicRobot.closeGame)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy\ h:mm"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -726,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -769,10 +783,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1096,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1120,10 +1133,10 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1613,36 +1626,36 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="27">
+      <c r="A29" s="26">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="24">
         <v>42000.640972222223</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="24">
         <v>42006.01666666667</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <v>42006.890277777777</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="27"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="28"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3">
@@ -1658,13 +1671,13 @@
       <c r="D32" s="5">
         <v>42008.844444444447</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>42010.81527777778</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3">
-        <f t="shared" ref="A33:A36" si="2">A32+1</f>
+        <f t="shared" ref="A33:A39" si="2">A32+1</f>
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -1673,28 +1686,28 @@
       <c r="C33" s="5">
         <v>42008.844444444447</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="1">
         <v>42010.817361111112</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>42011.962500000001</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="3">
+      <c r="A34" s="6">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="7">
         <v>42008.844444444447</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="7">
         <v>42011.99722222222</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="7">
         <v>42013.111111111109</v>
       </c>
     </row>
@@ -1703,13 +1716,136 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="1">
+        <v>42013.770138888889</v>
+      </c>
+      <c r="D35" s="1">
+        <v>42013.770138888889</v>
+      </c>
+      <c r="E35" s="1">
+        <v>42013.80972222222</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1">
+        <v>42013.770138888889</v>
+      </c>
+      <c r="D36" s="1">
+        <v>42013.80972222222</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="1">
+        <v>42013.770138888889</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="1">
+        <v>42013.770138888889</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="1">
+        <v>42013.770138888889</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="4:5">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="4:5">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="4:5">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
TASK_33, robot can do move
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>№</t>
   </si>
@@ -603,6 +603,9 @@
   </si>
   <si>
     <t>5.5 – Покинуть и игру с роботом. (LogicRobot.closeGame)</t>
+  </si>
+  <si>
+    <t>При создании пользователя, отправлять обновление друзей его онлайн друзьям.</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1862,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2077,6 +2080,14 @@
         <v>41988.625694444447</v>
       </c>
     </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="2">
+        <v>42013.963194444441</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TASK_34 finished, AIDoMove completed!
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>№</t>
   </si>
@@ -606,6 +606,9 @@
   </si>
   <si>
     <t>При создании пользователя, отправлять обновление друзей его онлайн друзьям.</t>
+  </si>
+  <si>
+    <t>Оптимизировать работу WebSocketClient, что бы создавал не более лимитного значения, коннектов, ато всё виснет.</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1118,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1746,7 +1749,9 @@
       <c r="D36" s="1">
         <v>42013.80972222222</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>42014.041666666664</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3">
@@ -1759,7 +1764,9 @@
       <c r="C37" s="1">
         <v>42013.770138888889</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1">
+        <v>42014.666666666664</v>
+      </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5">
@@ -1865,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2088,6 +2095,14 @@
         <v>42013.963194444441</v>
       </c>
     </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="2">
+        <v>42014.92083333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TASK_35, robot game closed and check winner.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>№</t>
   </si>
@@ -599,16 +599,14 @@
     <t>5.3 – Мозг робота. (LogicRobot.AIDoMove#2)</t>
   </si>
   <si>
-    <t>5.4 – Проверка победителя. (LogicRobot.checkWinner)</t>
-  </si>
-  <si>
-    <t>5.5 – Покинуть и игру с роботом. (LogicRobot.closeGame)</t>
-  </si>
-  <si>
     <t>При создании пользователя, отправлять обновление друзей его онлайн друзьям.</t>
   </si>
   <si>
     <t>Оптимизировать работу WebSocketClient, что бы создавал не более лимитного значения, коннектов, ато всё виснет.</t>
+  </si>
+  <si>
+    <t>5.4 – Проверка победителя. (LogicRobot.checkWinner)
+5.5 – Покинуть и игру с роботом. (LogicRobot.closeGame)</t>
   </si>
 </sst>
 </file>
@@ -746,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -812,6 +810,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
@@ -1767,33 +1768,30 @@
       <c r="D37" s="1">
         <v>42014.666666666664</v>
       </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="3">
+      <c r="E37" s="1">
+        <v>42014.952777777777</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" s="6">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="B38" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="7">
         <v>42013.770138888889</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="D38" s="7">
+        <v>42014.952777777777</v>
+      </c>
+      <c r="E38" s="7">
+        <v>42015.051388888889</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="3">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="1">
-        <v>42013.770138888889</v>
-      </c>
+      <c r="A39" s="3"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
@@ -1874,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2089,7 +2087,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2">
         <v>42013.963194444441</v>
@@ -2097,7 +2095,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="2">
         <v>42014.92083333333</v>

</xml_diff>

<commit_message>
some modifications of Config policy
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
     <sheet name="Бэклог задач" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>№</t>
   </si>
@@ -607,16 +607,25 @@
   <si>
     <t>5.4 – Проверка победителя. (LogicRobot.checkWinner)
 5.5 – Покинуть и игру с роботом. (LogicRobot.closeGame)</t>
+  </si>
+  <si>
+    <t>9.1 - На элемент Фото игрока добавим иконку пригласить, и мини кнопку "играем?". (elementPlayer#2)</t>
+  </si>
+  <si>
+    <t>9.2 - Функционал отправки приглашения. (LogicInvites.send)</t>
+  </si>
+  <si>
+    <t>9.3 - Функционал принятия приглашения. (LogicInvites.accept)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,6 +799,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -810,9 +822,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,7 +883,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -906,9 +915,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,6 +950,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1115,22 +1126,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1164,7 +1175,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -1182,7 +1193,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1200,7 +1211,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1218,7 +1229,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1236,7 +1247,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1254,7 +1265,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1272,7 +1283,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1290,7 +1301,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1308,7 +1319,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f>A10+1</f>
         <v>10</v>
@@ -1326,7 +1337,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1344,7 +1355,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1362,7 +1373,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1380,7 +1391,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1398,7 +1409,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1416,7 +1427,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1434,7 +1445,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1452,7 +1463,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1470,7 +1481,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1488,7 +1499,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1506,7 +1517,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1524,7 +1535,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1542,7 +1553,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1560,7 +1571,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1578,7 +1589,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1596,7 +1607,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1614,7 +1625,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1632,39 +1643,39 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="26">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="27">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="25">
         <v>42000.640972222223</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="25">
         <v>42006.01666666667</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="25">
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="26"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="27"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-    </row>
-    <row r="32" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f>A29+1</f>
         <v>29</v>
@@ -1682,9 +1693,9 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <f t="shared" ref="A33:A39" si="2">A32+1</f>
+        <f t="shared" ref="A33:A43" si="2">A32+1</f>
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -1700,7 +1711,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1718,7 +1729,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1736,7 +1747,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1754,7 +1765,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1772,12 +1783,12 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="21" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="7">
@@ -1790,68 +1801,107 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="3"/>
-      <c r="D39" s="1"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1">
+        <v>42016.468055555553</v>
+      </c>
+      <c r="D39" s="1">
+        <v>42016.468055555553</v>
+      </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="1">
+        <v>42016.468055555553</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="1">
+        <v>42016.468055555553</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="4:5">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="4:5">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="4:5">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="4:5">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="4:5">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="4:5">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
@@ -1869,21 +1919,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="72.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>10</v>
       </c>
@@ -1897,7 +1947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -1905,7 +1955,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1913,7 +1963,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1921,7 +1971,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -1929,7 +1979,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1937,7 +1987,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1945,7 +1995,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -1953,7 +2003,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1961,7 +2011,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -1969,7 +2019,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1977,7 +2027,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1985,7 +2035,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1993,7 +2043,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2013,7 +2063,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>33</v>
       </c>
@@ -2021,7 +2071,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -2029,7 +2079,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -2037,7 +2087,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -2045,7 +2095,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -2053,7 +2103,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>47</v>
       </c>
@@ -2061,7 +2111,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>48</v>
       </c>
@@ -2069,7 +2119,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>49</v>
       </c>
@@ -2077,7 +2127,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>51</v>
       </c>
@@ -2085,7 +2135,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>67</v>
       </c>
@@ -2093,7 +2143,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
TASK_36, completed, icons on photo added(invite,waiting,letsplay)
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1130,7 +1130,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1815,9 @@
       <c r="D39" s="1">
         <v>42016.468055555553</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1">
+        <v>42017.60833333333</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">

</xml_diff>

<commit_message>
TASK_37, finished. sendInvites, receiveInvites, LogicTimers realized
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1130,7 +1130,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,8 +1830,12 @@
       <c r="C40" s="1">
         <v>42016.468055555553</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="D40" s="1">
+        <v>42017.61041666667</v>
+      </c>
+      <c r="E40" s="1">
+        <v>42017.772222222222</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
@@ -1844,7 +1848,9 @@
       <c r="C41" s="1">
         <v>42016.468055555553</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1">
+        <v>42017.772222222222</v>
+      </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TASK_38, finished, invite game created now! is it realized! wow!:)
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>№</t>
   </si>
@@ -616,6 +616,33 @@
   </si>
   <si>
     <t>9.3 - Функционал принятия приглашения. (LogicInvites.accept)</t>
+  </si>
+  <si>
+    <t>Добавить поясняющие сообщение для DB, в случае если невозможно подключиться, сообщить о конфиге и т.д.</t>
+  </si>
+  <si>
+    <t>Добавить поясняющие сообщение для WebSocketServer, в случае если невозможно подключиться, сообщить о конфиге и т.д., занятости 80 порта(skype,apache?)</t>
+  </si>
+  <si>
+    <t>Вынести конфиг клиента в отдельный файл.</t>
+  </si>
+  <si>
+    <t>Поменять в photoInfo .id на userId. Ибо id  не фото, а юзера.</t>
+  </si>
+  <si>
+    <t>При создании игры по приглашению, если юзер оффлайн, нужно сообщить клиенту, что триндец, иначе так и будет висеть в ожидании игры.</t>
+  </si>
+  <si>
+    <t>Фотографию оппонента вывести</t>
+  </si>
+  <si>
+    <t>Для игры по приглашению учесть знак обоих игроков, а не только одного.</t>
+  </si>
+  <si>
+    <t>Рефакторинг: разделить random, robot and invitation game.</t>
+  </si>
+  <si>
+    <t>9.4 – Функционал состояния пользователя. (APIUserState)</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1157,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,14 +1878,24 @@
       <c r="D41" s="1">
         <v>42017.772222222222</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="1">
+        <v>42018.723611111112</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="1">
+        <v>42018.723611111112</v>
+      </c>
+      <c r="D42" s="1">
+        <v>42018.723611111112</v>
+      </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1928,16 +1965,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2159,6 +2196,70 @@
         <v>42014.92083333333</v>
       </c>
     </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2">
+        <v>42018.599305555559</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="2">
+        <v>42018.599305555559</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="2">
+        <v>42018.599305555559</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="2">
+        <v>42018.623611111114</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="2">
+        <v>42018.640972222223</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="2">
+        <v>42018.645138888889</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2">
+        <v>42018.645833333336</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="2">
+        <v>42018.697916666664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TASK_39, finished UserState realized!
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>№</t>
   </si>
@@ -643,6 +643,27 @@
   </si>
   <si>
     <t>9.4 – Функционал состояния пользователя. (APIUserState)</t>
+  </si>
+  <si>
+    <t>LogicUser.sendToAll, отправляет всем,  в некоторых случаях это не нужно,т.к. пользователь рассылает сообщие сам себе, надо проанализировать и устранить такую хренотеньку)</t>
+  </si>
+  <si>
+    <t>10.1 – Элемент список рейтинга. (elementRatingList)</t>
+  </si>
+  <si>
+    <t>10.2 – таблица рейтинга. (DB.rating)</t>
+  </si>
+  <si>
+    <t>10.3 – Обновление рейтинга на клиенте. (LogicRating.updateRating)</t>
+  </si>
+  <si>
+    <t>10.4 – Расчёт рейтинга. (LogicRating.calculateRating)</t>
+  </si>
+  <si>
+    <t>при onBusy удалюятся приглашения, но не таймеры, таймеры остаются, надо это исправить, мелочь, а приятно.</t>
+  </si>
+  <si>
+    <t>Доработотать sendMeUserInfo, кроме отправки online, нужно отправлять onGameId, isBusy, особено isBusy!</t>
   </si>
 </sst>
 </file>
@@ -780,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -829,6 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1156,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,36 +1693,36 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+      <c r="A29" s="28">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="26">
         <v>42000.640972222223</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="26">
         <v>42006.01666666667</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="26">
         <v>42006.890277777777</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1722,7 +1744,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <f t="shared" ref="A33:A43" si="2">A32+1</f>
+        <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -1883,70 +1905,121 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="A42" s="6">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="7">
         <v>42018.723611111112</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="7">
         <v>42018.723611111112</v>
       </c>
-      <c r="E42" s="1"/>
+      <c r="E42" s="7">
+        <v>42019.777083333334</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
+      <c r="B43" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="9">
+        <v>42019.77847222222</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="5">
+        <v>42019.77847222222</v>
+      </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="5">
+        <v>42019.77847222222</v>
+      </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="5">
+        <v>42019.77847222222</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="C47" s="5"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
@@ -1965,10 +2038,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,6 +2333,30 @@
         <v>42018.697916666664</v>
       </c>
     </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="2">
+        <v>42019.70208333333</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="2">
+        <v>42019.780555555553</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="2">
+        <v>42019.782638888886</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TASK_41, finished, rating table created
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -807,6 +807,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -834,7 +835,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1657,36 +1657,36 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36">
+      <c r="A29" s="37">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="33">
         <v>42000.640972222223</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="33">
         <v>42006.01666666667</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="35">
         <v>42006.890277777777</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="34"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="35"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="35"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
@@ -1897,7 +1897,7 @@
       <c r="C43" s="16">
         <v>42019.77847222222</v>
       </c>
-      <c r="D43" s="38">
+      <c r="D43" s="29">
         <v>42019.784722222219</v>
       </c>
       <c r="E43" s="16">
@@ -1918,7 +1918,9 @@
       <c r="D44" s="12">
         <v>42020.709722222222</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="12">
+        <v>42020.720138888886</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
@@ -1931,7 +1933,9 @@
       <c r="C45" s="12">
         <v>42019.77847222222</v>
       </c>
-      <c r="D45" s="12"/>
+      <c r="D45" s="12">
+        <v>42020.720138888886</v>
+      </c>
       <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
TASK_42, completed, rating realy loading right now, mmm...
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>№</t>
   </si>
@@ -637,6 +637,18 @@
   </si>
   <si>
     <t>10.2 – Таблица рейтинга. (DB.rating)</t>
+  </si>
+  <si>
+    <t>Оптимизировать загрузку рейтинга. Сейчас при заходе на страницу рейтинга, обновляется каждую секунду, в т.ч. Данные очков берутьс из юзера, а вот позиции могут не соответстовать.</t>
+  </si>
+  <si>
+    <t>Сделать заголовок рейтингу. Его нет, а это печально, прям жесть, без этого нельзя запускать.</t>
+  </si>
+  <si>
+    <t>Добавить рейтинг по друзьям.</t>
+  </si>
+  <si>
+    <t>Добавить рейтинг по позиции игрока.</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1154,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1936,7 +1948,9 @@
       <c r="D45" s="12">
         <v>42020.720138888886</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="E45" s="12">
+        <v>42020.774305555555</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="26">
@@ -1949,7 +1963,9 @@
       <c r="C46" s="28">
         <v>42019.77847222222</v>
       </c>
-      <c r="D46" s="28"/>
+      <c r="D46" s="12">
+        <v>42020.774305555555</v>
+      </c>
       <c r="E46" s="28"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2012,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,6 +2355,38 @@
         <v>42020.539583333331</v>
       </c>
     </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="2">
+        <v>42020.765972222223</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="2">
+        <v>42020.76666666667</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="2">
+        <v>42020.767361111109</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="2">
+        <v>42020.767361111109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TASK_43, finished, rating updated after users score up.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>№</t>
   </si>
@@ -649,6 +649,18 @@
   </si>
   <si>
     <t>Добавить рейтинг по позиции игрока.</t>
+  </si>
+  <si>
+    <t>Добавить обновление rating.updated, при обновлении позиции.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сделать логирование по id класса! </t>
+  </si>
+  <si>
+    <t>Сделать логирование по id сообщения!</t>
+  </si>
+  <si>
+    <t>Организовать событийнные механизмы. Ато как то евент вызыаются прямыми обращениями в методы.</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -2028,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,6 +2399,38 @@
         <v>42020.767361111109</v>
       </c>
     </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="2">
+        <v>42023.718055555553</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="2">
+        <v>42023.720138888886</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="2">
+        <v>42023.720138888886</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="2">
+        <v>42023.724999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Highload functional begining, The Krispi robot.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>№</t>
   </si>
@@ -669,17 +669,20 @@
     <t>Сливание кэша чата какое то не правильное, сливется всё, но в кэше остается почти столькоже, результат дублирование.</t>
   </si>
   <si>
-    <t>Отображать на ленте свободных. онлайн юзеров!</t>
+    <t>Система перезапуска сервера.</t>
+  </si>
+  <si>
+    <t>Система постоянного таймаут-пинга, с оповещением.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -945,7 +948,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,10 +980,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1012,7 +1014,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1188,14 +1189,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1204,7 +1205,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1256,7 +1257,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1274,7 +1275,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1292,7 +1293,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1310,7 +1311,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1328,7 +1329,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1346,7 +1347,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1364,7 +1365,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1382,7 +1383,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1400,7 +1401,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1418,7 +1419,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1436,7 +1437,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1454,7 +1455,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1472,7 +1473,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1490,7 +1491,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1508,7 +1509,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1526,7 +1527,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1544,7 +1545,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1562,7 +1563,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1580,7 +1581,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1598,7 +1599,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1616,7 +1617,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1634,7 +1635,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1652,7 +1653,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1670,7 +1671,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1688,7 +1689,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1706,7 +1707,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="35">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1724,21 +1725,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="35"/>
       <c r="B30" s="29"/>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
       <c r="E30" s="33"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="36"/>
       <c r="B31" s="30"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="34"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1756,7 +1757,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1774,7 +1775,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1792,7 +1793,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1810,7 +1811,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1828,7 +1829,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1846,7 +1847,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1864,7 +1865,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1882,7 +1883,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1900,7 +1901,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1918,7 +1919,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -1936,7 +1937,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -1954,7 +1955,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -1972,7 +1973,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -1990,7 +1991,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2008,7 +2009,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2017,7 +2018,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2025,7 +2026,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2033,23 +2034,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2067,21 +2068,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="153.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2127,7 +2128,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2151,7 +2152,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -2219,7 +2220,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2251,7 +2252,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2299,7 +2300,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2339,7 +2340,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
         <v>62</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2419,7 +2420,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2427,7 +2428,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2435,7 +2436,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2459,7 +2460,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2467,12 +2468,20 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3">
       <c r="B47" t="s">
         <v>99</v>
       </c>
       <c r="C47" s="2">
-        <v>42032.820833333331</v>
+        <v>42035.98333333333</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="2">
+        <v>42035.98333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some profiler points, Krispi level up.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>№</t>
   </si>
@@ -673,16 +673,34 @@
   </si>
   <si>
     <t>Система постоянного таймаут-пинга, с оповещением.</t>
+  </si>
+  <si>
+    <t>Постинг нша стену результатов игры.</t>
+  </si>
+  <si>
+    <t>Оптимизация: индексы для users.socNetTypeId и users.socNetUserId</t>
+  </si>
+  <si>
+    <t>Оптимизация: кэширование для запросов к социальной сети! В первую очередь это нужно для тестирования, т.к. мы просто замучаем АПИ соц сети,  не хорошо это, вот.</t>
+  </si>
+  <si>
+    <t>Рейтинг пытается отобразить английские буквы, failed</t>
+  </si>
+  <si>
+    <t>ElementGraphicsText если нет картинки символа - заменять на текст.</t>
+  </si>
+  <si>
+    <t>При  закрытие клиента, похоже, что его игры не закрываются, а остаются в статусе 2!, если это так, соответствено добавить на это тест.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -948,7 +966,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -980,9 +998,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1014,6 +1033,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1189,14 +1209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1205,7 +1225,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1239,7 +1259,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1257,7 +1277,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1275,7 +1295,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1293,7 +1313,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1311,7 +1331,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1329,7 +1349,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1347,7 +1367,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1365,7 +1385,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1383,7 +1403,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1401,7 +1421,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1419,7 +1439,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1437,7 +1457,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1455,7 +1475,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1473,7 +1493,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1491,7 +1511,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1509,7 +1529,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1527,7 +1547,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1545,7 +1565,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1563,7 +1583,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1581,7 +1601,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1599,7 +1619,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1617,7 +1637,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1635,7 +1655,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1653,7 +1673,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1671,7 +1691,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1689,7 +1709,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1707,7 +1727,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1725,21 +1745,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="35"/>
       <c r="B30" s="29"/>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
       <c r="E30" s="33"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
       <c r="B31" s="30"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="34"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1757,7 +1777,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1775,7 +1795,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1793,7 +1813,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1811,7 +1831,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1829,7 +1849,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1847,7 +1867,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1865,7 +1885,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1883,7 +1903,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1901,7 +1921,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1919,7 +1939,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -1937,7 +1957,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -1955,7 +1975,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -1973,7 +1993,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -1991,7 +2011,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2009,7 +2029,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2018,7 +2038,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2026,7 +2046,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2034,23 +2054,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2068,21 +2088,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="153.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2096,7 +2116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -2104,7 +2124,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2112,7 +2132,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2120,7 +2140,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2128,7 +2148,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2136,7 +2156,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -2144,7 +2164,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2152,7 +2172,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2160,7 +2180,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2168,7 +2188,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -2176,7 +2196,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2184,7 +2204,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -2192,7 +2212,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2212,7 +2232,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -2220,7 +2240,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -2228,7 +2248,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -2236,7 +2256,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -2244,7 +2264,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2252,7 +2272,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2260,7 +2280,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2268,7 +2288,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2276,7 +2296,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2284,7 +2304,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2292,7 +2312,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2300,7 +2320,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2308,7 +2328,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2316,7 +2336,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2324,7 +2344,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2332,7 +2352,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2340,7 +2360,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>62</v>
       </c>
@@ -2348,7 +2368,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2356,7 +2376,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2364,7 +2384,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2372,7 +2392,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2380,7 +2400,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2388,7 +2408,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2396,7 +2416,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2404,7 +2424,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2412,7 +2432,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2420,7 +2440,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2428,7 +2448,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2436,7 +2456,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2444,7 +2464,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2452,7 +2472,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2460,7 +2480,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2468,7 +2488,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>99</v>
       </c>
@@ -2476,7 +2496,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>100</v>
       </c>
@@ -2484,7 +2504,56 @@
         <v>42035.98333333333</v>
       </c>
     </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="2">
+        <v>42037.756944444445</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="2">
+        <v>42038.629861111112</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="2">
+        <v>42038.629861111112</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="2">
+        <v>42038.938888888886</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="2">
+        <v>42038.950694444444</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="2">
+        <v>42039.758333333331</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I think Krispi highload completed!
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>№</t>
   </si>
@@ -697,6 +697,9 @@
   </si>
   <si>
     <t>System.clientCodeAutoReload(boolean);</t>
+  </si>
+  <si>
+    <t>проверить все WHERE_IN, баг пролазел , хотя проверка есть на undefined</t>
   </si>
 </sst>
 </file>
@@ -706,7 +709,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,6 +731,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -810,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -884,6 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2093,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2572,6 +2583,14 @@
         <v>42040.088194444441</v>
       </c>
     </row>
+    <row r="57" spans="2:3" ht="15.75">
+      <c r="B57" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="2">
+        <v>42040.129861111112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Opponent photo. Add friends dialog button.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>№</t>
   </si>
@@ -700,6 +700,21 @@
   </si>
   <si>
     <t>проверить все WHERE_IN, баг пролазел , хотя проверка есть на undefined</t>
+  </si>
+  <si>
+    <t>вынести ID_* профайлера в отедельный файл</t>
+  </si>
+  <si>
+    <t>GUIDom not selectable by default</t>
+  </si>
+  <si>
+    <t>Рейтинг не верно отображается(сортировка?!)</t>
+  </si>
+  <si>
+    <t>Рейтинг перекрывает онлайн и очки</t>
+  </si>
+  <si>
+    <t>ElementPhoto - effect old photo like-a</t>
   </si>
 </sst>
 </file>
@@ -867,6 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -894,7 +910,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1743,36 +1758,36 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="35">
+      <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="31">
+      <c r="C29" s="32">
         <v>42000.640972222223</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="32">
         <v>42006.01666666667</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="34">
         <v>42006.890277777777</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="35"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="33"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="36"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="34"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="35"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
@@ -2104,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2584,11 +2599,48 @@
       </c>
     </row>
     <row r="57" spans="2:3" ht="15.75">
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="28" t="s">
         <v>109</v>
       </c>
       <c r="C57" s="2">
         <v>42040.129861111112</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="2">
+        <v>42040.138888888891</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="2">
+        <v>42040.140277777777</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="2">
+        <v>42040.140277777777</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" s="2">
+        <v>42040.140277777777</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Repeat game realized, and some little fix-bugs
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>№</t>
   </si>
@@ -715,16 +715,28 @@
   </si>
   <si>
     <t>ElementPhoto - effect old photo like-a</t>
+  </si>
+  <si>
+    <t>3 на 3 уехали нулики</t>
+  </si>
+  <si>
+    <t>15 на 15 ухала линияпобеды слева на право вверх.</t>
+  </si>
+  <si>
+    <t>При повторе игры, кто выиграл тот и крестик.</t>
+  </si>
+  <si>
+    <t>прятать кнопку "Еще" если игрок покинул игру.onGame(0)?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,7 +1010,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1030,9 +1042,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1064,6 +1077,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1239,14 +1253,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1255,7 +1269,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1289,7 +1303,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1307,7 +1321,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1325,7 +1339,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1343,7 +1357,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1361,7 +1375,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1379,7 +1393,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1397,7 +1411,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1415,7 +1429,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1433,7 +1447,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1451,7 +1465,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1469,7 +1483,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1487,7 +1501,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1505,7 +1519,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1523,7 +1537,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1541,7 +1555,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1559,7 +1573,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1577,7 +1591,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1595,7 +1609,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1613,7 +1627,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1631,7 +1645,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1649,7 +1663,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1667,7 +1681,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1685,7 +1699,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1703,7 +1717,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1721,7 +1735,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1739,7 +1753,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1757,7 +1771,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1775,21 +1789,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1807,7 +1821,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1825,7 +1839,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1843,7 +1857,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1861,7 +1875,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1879,7 +1893,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1897,7 +1911,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1915,7 +1929,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1933,7 +1947,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1951,7 +1965,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1969,7 +1983,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -1987,7 +2001,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2005,7 +2019,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2023,7 +2037,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2041,7 +2055,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2059,7 +2073,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2068,7 +2082,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2076,7 +2090,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2084,23 +2098,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2118,21 +2132,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2146,7 +2160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2168,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2162,7 +2176,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2170,7 +2184,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2178,7 +2192,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2186,7 +2200,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -2194,7 +2208,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2202,7 +2216,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2210,7 +2224,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2218,7 +2232,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -2226,7 +2240,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2234,7 +2248,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -2242,7 +2256,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2262,7 +2276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -2270,7 +2284,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -2278,7 +2292,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -2286,7 +2300,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -2294,7 +2308,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2302,7 +2316,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2310,7 +2324,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2318,7 +2332,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2326,7 +2340,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2334,7 +2348,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2342,7 +2356,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2350,7 +2364,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2358,7 +2372,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2366,7 +2380,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2374,7 +2388,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2382,7 +2396,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2390,7 +2404,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>62</v>
       </c>
@@ -2398,7 +2412,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2406,7 +2420,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2414,7 +2428,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2422,7 +2436,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2430,7 +2444,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2438,7 +2452,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2446,7 +2460,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2454,7 +2468,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2462,7 +2476,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2470,7 +2484,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2478,7 +2492,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2486,7 +2500,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2494,7 +2508,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2502,7 +2516,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2510,7 +2524,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2518,7 +2532,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>99</v>
       </c>
@@ -2526,7 +2540,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>100</v>
       </c>
@@ -2534,7 +2548,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>101</v>
       </c>
@@ -2542,7 +2556,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>102</v>
       </c>
@@ -2550,7 +2564,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>103</v>
       </c>
@@ -2558,7 +2572,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>104</v>
       </c>
@@ -2566,7 +2580,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="53" spans="2:3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>105</v>
       </c>
@@ -2574,7 +2588,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="54" spans="2:3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>106</v>
       </c>
@@ -2582,7 +2596,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="55" spans="2:3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>107</v>
       </c>
@@ -2590,7 +2604,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="56" spans="2:3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>108</v>
       </c>
@@ -2598,7 +2612,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="15.75">
+    <row r="57" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
         <v>109</v>
       </c>
@@ -2606,7 +2620,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="58" spans="2:3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>110</v>
       </c>
@@ -2614,7 +2628,7 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="59" spans="2:3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>111</v>
       </c>
@@ -2622,7 +2636,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="60" spans="2:3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>112</v>
       </c>
@@ -2630,7 +2644,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="61" spans="2:3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>113</v>
       </c>
@@ -2638,9 +2652,29 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="62" spans="2:3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All users on Friend type
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>№</t>
   </si>
@@ -727,6 +727,9 @@
   </si>
   <si>
     <t>прятать кнопку "Еще" если игрок покинул игру.onGame(0)?</t>
+  </si>
+  <si>
+    <t>надо подгружать тех, кто сейчас являются онлайн</t>
   </si>
 </sst>
 </file>
@@ -2133,10 +2136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,6 +2680,11 @@
         <v>118</v>
       </c>
     </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add scoreonline page and so on so on and so on and so and on
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="120">
   <si>
     <t>№</t>
   </si>
@@ -669,9 +669,6 @@
     <t>Сливание кэша чата какое то не правильное, сливется всё, но в кэше остается почти столькоже, результат дублирование.</t>
   </si>
   <si>
-    <t>Система перезапуска сервера.</t>
-  </si>
-  <si>
     <t>Система постоянного таймаут-пинга, с оповещением.</t>
   </si>
   <si>
@@ -730,16 +727,19 @@
   </si>
   <si>
     <t>надо подгружать тех, кто сейчас являются онлайн</t>
+  </si>
+  <si>
+    <t>Система автозапуска сервера.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,7 +1013,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1045,10 +1045,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1080,7 +1079,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1256,14 +1254,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1272,7 +1270,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1306,7 +1304,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1324,7 +1322,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1342,7 +1340,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1360,7 +1358,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1378,7 +1376,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1396,7 +1394,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1414,7 +1412,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1432,7 +1430,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1450,7 +1448,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1468,7 +1466,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1486,7 +1484,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1504,7 +1502,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1522,7 +1520,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1540,7 +1538,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1558,7 +1556,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1576,7 +1574,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1594,7 +1592,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1612,7 +1610,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1630,7 +1628,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1648,7 +1646,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1666,7 +1664,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1684,7 +1682,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1702,7 +1700,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1720,7 +1718,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1738,7 +1736,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1756,7 +1754,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1774,7 +1772,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1792,21 +1790,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1824,7 +1822,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1842,7 +1840,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1860,7 +1858,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1878,7 +1876,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1896,7 +1894,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1914,7 +1912,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1932,7 +1930,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1950,7 +1948,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1968,7 +1966,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1986,7 +1984,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2004,7 +2002,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2022,7 +2020,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2040,7 +2038,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2058,7 +2056,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2076,7 +2074,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2085,7 +2083,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2093,7 +2091,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2101,23 +2099,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2135,21 +2133,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2169,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2179,7 +2177,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2187,7 +2185,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2195,7 +2193,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2203,7 +2201,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -2211,7 +2209,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2219,7 +2217,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +2225,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2251,7 +2249,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -2259,7 +2257,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2279,7 +2277,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -2287,7 +2288,10 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -2295,7 +2299,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -2303,7 +2307,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -2311,7 +2315,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2327,7 +2331,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2335,7 +2339,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2343,7 +2347,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2351,7 +2355,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2359,7 +2363,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2367,7 +2371,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2375,7 +2379,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2383,7 +2387,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2391,7 +2395,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2399,7 +2403,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2407,7 +2411,10 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
@@ -2415,7 +2422,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2423,7 +2430,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2431,7 +2438,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2439,7 +2446,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2447,7 +2454,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2455,7 +2462,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2463,7 +2470,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2479,7 +2486,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2487,7 +2494,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2495,7 +2502,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2503,7 +2510,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2511,7 +2518,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2519,7 +2526,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2527,7 +2534,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2535,158 +2542,164 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C47" s="2">
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="B48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2">
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2">
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2">
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="B51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C51" s="2">
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="B52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C52" s="2">
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="B53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C53" s="2">
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="B54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C54" s="2">
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="B55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C55" s="2">
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="B56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C56" s="2">
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15.75">
       <c r="B57" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C57" s="2">
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="B58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C58" s="2">
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="B59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C59" s="2">
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="B60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C60" s="2">
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="B61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C61" s="2">
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="B62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="B63" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="64" spans="1:3">
+      <c r="B64" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
image cache, add help page(first)
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="124">
   <si>
     <t>№</t>
   </si>
@@ -730,16 +730,28 @@
   </si>
   <si>
     <t>Система автозапуска сервера.</t>
+  </si>
+  <si>
+    <t>GUI.createElement, аргумент name превратить из string в objectName</t>
+  </si>
+  <si>
+    <t>сделать один метод вместо var el = GUI.create(name, params) self.els.push(el); сделать createelement(name,params); да..было бы круто)</t>
+  </si>
+  <si>
+    <t>В PageHelp для elementText реализовать клик, такой же как у checkbox-а напротив этого текста.</t>
+  </si>
+  <si>
+    <t>метод initMainMenuTab создаёт картинки с opacity,возможно, надо доработать ElementImage.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,7 +1025,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1045,9 +1057,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1079,6 +1092,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1254,14 +1268,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1270,7 +1284,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1304,7 +1318,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1322,7 +1336,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1340,7 +1354,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1358,7 +1372,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1376,7 +1390,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1394,7 +1408,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1412,7 +1426,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1430,7 +1444,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1448,7 +1462,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1466,7 +1480,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1484,7 +1498,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1502,7 +1516,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1520,7 +1534,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1538,7 +1552,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1556,7 +1570,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1574,7 +1588,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1592,7 +1606,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1610,7 +1624,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1628,7 +1642,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1646,7 +1660,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1664,7 +1678,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1682,7 +1696,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1700,7 +1714,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1718,7 +1732,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1736,7 +1750,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1754,7 +1768,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1772,7 +1786,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1790,21 +1804,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1822,7 +1836,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1840,7 +1854,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1858,7 +1872,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1876,7 +1890,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1894,7 +1908,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1912,7 +1926,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1930,7 +1944,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1948,7 +1962,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1966,7 +1980,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1984,7 +1998,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2002,7 +2016,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2020,7 +2034,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2038,7 +2052,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2056,7 +2070,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2074,7 +2088,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2083,7 +2097,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2091,7 +2105,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2099,23 +2113,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2133,21 +2147,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2161,7 +2175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -2169,7 +2183,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2177,7 +2191,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2185,7 +2199,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2207,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2201,7 +2215,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -2209,7 +2223,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2217,7 +2231,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2225,7 +2239,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2233,7 +2247,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -2241,7 +2255,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2249,7 +2263,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -2257,7 +2271,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2277,7 +2291,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2288,7 +2302,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2299,7 +2313,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -2307,7 +2321,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -2315,7 +2329,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2323,7 +2337,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2331,7 +2345,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2339,7 +2353,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2347,7 +2361,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2355,7 +2369,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2363,7 +2377,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2371,7 +2385,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2379,7 +2393,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2387,7 +2401,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2395,7 +2409,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2403,7 +2417,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2411,7 +2425,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2422,7 +2436,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2430,7 +2444,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2438,7 +2452,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2446,7 +2460,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2454,7 +2468,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2462,7 +2476,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2470,7 +2484,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2478,7 +2492,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2486,7 +2500,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2494,7 +2508,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2502,7 +2516,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2510,7 +2524,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2518,7 +2532,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2526,7 +2540,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2534,7 +2548,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2542,7 +2556,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2553,7 +2567,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>99</v>
       </c>
@@ -2561,7 +2575,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>100</v>
       </c>
@@ -2569,7 +2583,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2580,7 +2594,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>102</v>
       </c>
@@ -2588,7 +2602,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>103</v>
       </c>
@@ -2596,7 +2610,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>104</v>
       </c>
@@ -2604,7 +2618,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>105</v>
       </c>
@@ -2612,7 +2626,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>106</v>
       </c>
@@ -2620,7 +2634,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>107</v>
       </c>
@@ -2628,7 +2642,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75">
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
         <v>108</v>
       </c>
@@ -2636,7 +2650,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>109</v>
       </c>
@@ -2644,7 +2658,7 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>110</v>
       </c>
@@ -2652,7 +2666,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>111</v>
       </c>
@@ -2660,7 +2674,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>112</v>
       </c>
@@ -2668,34 +2682,54 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix ElementText fatal but, and realize PageHelpRating.
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="125">
   <si>
     <t>№</t>
   </si>
@@ -742,6 +742,9 @@
   </si>
   <si>
     <t>метод initMainMenuTab создаёт картинки с opacity,возможно, надо доработать ElementImage.</t>
+  </si>
+  <si>
+    <t>На странице рейтинга, подогонать углы фотографий, лдумаю сделать их непоменьше.</t>
   </si>
 </sst>
 </file>
@@ -2148,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,6 +2735,11 @@
         <v>123</v>
       </c>
     </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
some develop some code
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
   <si>
     <t>№</t>
   </si>
@@ -791,15 +791,24 @@
   <si>
     <t>passphare убрать как то</t>
   </si>
+  <si>
+    <t>Запретить на "бою" робота криспи.</t>
+  </si>
+  <si>
+    <t>убрать рут права из коносли, ато уже ребутнул плин)</t>
+  </si>
+  <si>
+    <t>зашел, второй клиент перезагрузил, есть кнопка "еще" , плин</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,7 +1082,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1105,10 +1114,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1140,7 +1148,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1316,14 +1323,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1332,7 +1339,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1366,7 +1373,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1384,7 +1391,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1402,7 +1409,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1420,7 +1427,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1438,7 +1445,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1456,7 +1463,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1474,7 +1481,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1492,7 +1499,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1510,7 +1517,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1528,7 +1535,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1546,7 +1553,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1564,7 +1571,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1582,7 +1589,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1600,7 +1607,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1618,7 +1625,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1636,7 +1643,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1654,7 +1661,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1672,7 +1679,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1690,7 +1697,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1708,7 +1715,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1726,7 +1733,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1744,7 +1751,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1762,7 +1769,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1780,7 +1787,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1798,7 +1805,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1816,7 +1823,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1834,7 +1841,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1852,21 +1859,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1884,7 +1891,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1902,7 +1909,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1920,7 +1927,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1938,7 +1945,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1956,7 +1963,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1974,7 +1981,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1992,7 +1999,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -2010,7 +2017,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -2028,7 +2035,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2046,7 +2053,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2064,7 +2071,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2082,7 +2089,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2100,7 +2107,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2118,7 +2125,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2136,7 +2143,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2148,7 +2155,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2156,7 +2163,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2164,23 +2171,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2198,21 +2205,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:B82"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2233,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2237,7 +2244,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -2248,7 +2255,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2259,7 +2266,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2267,7 +2274,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2275,7 +2282,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -2286,7 +2293,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -2297,7 +2304,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2305,7 +2312,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2313,7 +2320,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2324,7 +2331,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -2335,7 +2342,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -2346,7 +2353,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2366,7 +2373,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2377,7 +2384,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2388,7 +2395,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -2399,7 +2406,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -2410,7 +2417,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2418,7 +2425,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2426,7 +2433,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2434,7 +2441,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2442,7 +2449,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2458,7 +2465,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2466,7 +2473,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2474,7 +2481,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2482,7 +2489,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2490,7 +2497,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2498,7 +2505,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2517,7 +2524,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2525,7 +2532,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2533,7 +2540,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2541,7 +2548,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2549,7 +2556,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2557,7 +2564,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2565,7 +2572,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2573,7 +2580,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2581,7 +2588,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2589,7 +2596,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2597,7 +2604,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2605,7 +2612,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2613,7 +2620,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2621,7 +2628,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2629,7 +2636,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2637,7 +2644,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2648,7 +2655,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="B48" t="s">
         <v>99</v>
       </c>
@@ -2656,7 +2663,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="B49" t="s">
         <v>100</v>
       </c>
@@ -2664,7 +2671,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2675,7 +2682,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="B51" t="s">
         <v>102</v>
       </c>
@@ -2683,7 +2690,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="B52" t="s">
         <v>103</v>
       </c>
@@ -2691,7 +2698,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="B53" t="s">
         <v>104</v>
       </c>
@@ -2699,7 +2706,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="B54" t="s">
         <v>105</v>
       </c>
@@ -2707,7 +2714,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="B55" t="s">
         <v>106</v>
       </c>
@@ -2715,7 +2722,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="B56" t="s">
         <v>107</v>
       </c>
@@ -2723,7 +2730,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15.75">
       <c r="B57" s="28" t="s">
         <v>108</v>
       </c>
@@ -2731,7 +2738,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="B58" t="s">
         <v>109</v>
       </c>
@@ -2739,7 +2746,7 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="B59" t="s">
         <v>110</v>
       </c>
@@ -2747,7 +2754,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -2758,7 +2765,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -2777,7 +2784,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -2785,7 +2792,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2793,52 +2800,52 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="B65" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="B66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="B67" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="B68" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="B69" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="B70" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="B71" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="B72" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="B73" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2846,7 +2853,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -2854,54 +2861,69 @@
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="B76" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="B77" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="B78" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="B79" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="B80" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2">
       <c r="B81" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2">
       <c r="B83" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2">
       <c r="B84" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2">
       <c r="B85" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2">
       <c r="B86" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hins and some fixes
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
   <si>
     <t>№</t>
   </si>
@@ -800,15 +800,21 @@
   <si>
     <t>зашел, второй клиент перезагрузил, есть кнопка "еще" , плин</t>
   </si>
+  <si>
+    <t>в конце каждого дива графического текста: function (l, c) {  return new Array(l - this.length + 1).join(c || '0') + this; }, Ubuntu Firefox (Илья Барышников)</t>
+  </si>
+  <si>
+    <t>hint-s всем кнопкам и прочим активным элементам.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,7 +1088,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1114,9 +1120,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1148,6 +1155,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1323,14 +1331,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1339,7 +1347,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1373,7 +1381,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1391,7 +1399,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1409,7 +1417,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1427,7 +1435,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1445,7 +1453,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1463,7 +1471,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1481,7 +1489,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1499,7 +1507,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1517,7 +1525,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1535,7 +1543,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1553,7 +1561,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1571,7 +1579,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1589,7 +1597,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1607,7 +1615,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1625,7 +1633,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1643,7 +1651,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1661,7 +1669,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1679,7 +1687,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1697,7 +1705,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1715,7 +1723,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1733,7 +1741,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1751,7 +1759,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1769,7 +1777,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1787,7 +1795,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1805,7 +1813,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1823,7 +1831,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1841,7 +1849,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1859,21 +1867,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1891,7 +1899,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1909,7 +1917,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1927,7 +1935,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1945,7 +1953,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1963,7 +1971,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1981,7 +1989,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1999,7 +2007,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -2017,7 +2025,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -2035,7 +2043,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2053,7 +2061,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2071,7 +2079,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2089,7 +2097,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2107,7 +2115,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2125,7 +2133,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2143,7 +2151,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2155,7 +2163,7 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2163,7 +2171,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2171,23 +2179,23 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2205,21 +2213,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2233,7 +2241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2244,7 +2252,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -2255,7 +2263,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2266,7 +2274,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -2274,7 +2282,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -2293,7 +2301,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -2304,7 +2312,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2312,7 +2320,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -2320,7 +2328,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2331,7 +2339,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -2342,7 +2350,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -2353,7 +2361,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2373,7 +2381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2384,7 +2392,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2395,7 +2403,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -2406,7 +2414,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -2417,7 +2425,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -2425,7 +2433,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -2433,7 +2441,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>38</v>
       </c>
@@ -2441,7 +2449,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -2449,7 +2457,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -2457,7 +2465,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -2465,7 +2473,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>52</v>
       </c>
@@ -2473,7 +2481,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>57</v>
       </c>
@@ -2481,7 +2489,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>58</v>
       </c>
@@ -2489,7 +2497,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -2497,7 +2505,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -2505,7 +2513,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>61</v>
       </c>
@@ -2513,7 +2521,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2524,7 +2532,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -2532,7 +2540,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2540,7 +2548,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -2548,7 +2556,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>70</v>
       </c>
@@ -2556,7 +2564,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>71</v>
       </c>
@@ -2564,7 +2572,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -2572,7 +2580,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2580,7 +2588,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2588,7 +2596,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>92</v>
       </c>
@@ -2596,7 +2604,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>93</v>
       </c>
@@ -2604,7 +2612,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>94</v>
       </c>
@@ -2612,7 +2620,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2620,7 +2628,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2628,7 +2636,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2636,7 +2644,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>98</v>
       </c>
@@ -2644,7 +2652,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2655,7 +2663,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>99</v>
       </c>
@@ -2663,7 +2671,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>100</v>
       </c>
@@ -2671,7 +2679,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2682,7 +2690,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>102</v>
       </c>
@@ -2690,7 +2698,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>103</v>
       </c>
@@ -2698,7 +2706,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>104</v>
       </c>
@@ -2706,7 +2714,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>105</v>
       </c>
@@ -2714,7 +2722,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>106</v>
       </c>
@@ -2722,7 +2730,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>107</v>
       </c>
@@ -2730,7 +2738,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75">
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
         <v>108</v>
       </c>
@@ -2738,7 +2746,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>109</v>
       </c>
@@ -2746,7 +2754,7 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>110</v>
       </c>
@@ -2754,7 +2762,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -2765,7 +2773,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -2776,7 +2784,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -2784,7 +2792,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -2792,7 +2800,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2800,52 +2808,52 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -2853,7 +2861,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -2861,69 +2869,79 @@
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="2:2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="2:2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="2:2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="2:2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="88" spans="2:2">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="2:2">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TASK_47, save user logout time
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="160">
   <si>
     <t>№</t>
   </si>
@@ -846,15 +846,21 @@
   <si>
     <t>Сделать фокус на вводе сообщения в чат.</t>
   </si>
+  <si>
+    <t>Новый рейтинг</t>
+  </si>
+  <si>
+    <t>Сохранять логаут юзера.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1128,7 +1134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1160,10 +1166,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1195,7 +1200,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1371,14 +1375,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1387,7 +1391,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +1408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1421,7 +1425,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1439,7 +1443,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1457,7 +1461,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1475,7 +1479,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1493,7 +1497,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1511,7 +1515,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1529,7 +1533,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1547,7 +1551,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1565,7 +1569,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1583,7 +1587,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1601,7 +1605,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1619,7 +1623,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1637,7 +1641,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1655,7 +1659,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1673,7 +1677,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1691,7 +1695,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1709,7 +1713,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1727,7 +1731,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1745,7 +1749,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1763,7 +1767,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1781,7 +1785,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1799,7 +1803,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1817,7 +1821,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1835,7 +1839,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1853,7 +1857,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1871,7 +1875,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1889,7 +1893,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1907,21 +1911,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1939,7 +1943,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1957,7 +1961,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1975,7 +1979,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1993,7 +1997,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -2011,7 +2015,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -2029,7 +2033,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -2047,7 +2051,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -2065,7 +2069,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -2083,7 +2087,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2101,7 +2105,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2119,7 +2123,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2137,7 +2141,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2155,7 +2159,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2173,7 +2177,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2191,7 +2195,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2209,7 +2213,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2220,31 +2224,40 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
+      <c r="B49" s="5" t="s">
+        <v>158</v>
+      </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A50" s="5">
+        <v>47</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2262,21 +2275,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2290,7 +2303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -2298,7 +2311,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -2306,7 +2319,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -2314,7 +2327,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -2322,7 +2335,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2333,7 +2346,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -2341,7 +2354,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -2349,7 +2362,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>41</v>
       </c>
@@ -2357,7 +2370,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -2365,7 +2378,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>57</v>
       </c>
@@ -2373,7 +2386,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>58</v>
       </c>
@@ -2381,7 +2394,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2392,7 +2405,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="B14" t="s">
         <v>60</v>
       </c>
@@ -2400,7 +2413,7 @@
         <v>42018.623611111114</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
         <v>63</v>
       </c>
@@ -2408,7 +2421,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>64</v>
       </c>
@@ -2416,7 +2429,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>66</v>
       </c>
@@ -2424,7 +2437,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
         <v>70</v>
       </c>
@@ -2432,7 +2445,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>88</v>
       </c>
@@ -2440,7 +2453,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="B20" t="s">
         <v>90</v>
       </c>
@@ -2448,7 +2461,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="B21" t="s">
         <v>92</v>
       </c>
@@ -2456,7 +2469,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="B22" t="s">
         <v>93</v>
       </c>
@@ -2464,7 +2477,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="B23" t="s">
         <v>94</v>
       </c>
@@ -2472,7 +2485,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="B24" t="s">
         <v>95</v>
       </c>
@@ -2480,7 +2493,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="B25" t="s">
         <v>96</v>
       </c>
@@ -2488,7 +2501,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>97</v>
       </c>
@@ -2496,7 +2509,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="B27" t="s">
         <v>99</v>
       </c>
@@ -2504,7 +2517,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>100</v>
       </c>
@@ -2512,7 +2525,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2523,7 +2536,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2534,7 +2547,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.75">
       <c r="B31" s="28" t="s">
         <v>107</v>
       </c>
@@ -2542,7 +2555,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="B32" t="s">
         <v>108</v>
       </c>
@@ -2550,12 +2563,12 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="B33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -2563,7 +2576,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -2571,17 +2584,17 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="B36" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="B37" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -2589,7 +2602,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -2597,7 +2610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2605,27 +2618,27 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="B41" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="B42" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="B43" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="B44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2633,7 +2646,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -2641,12 +2654,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="B47" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -2654,12 +2667,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="B49" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2667,47 +2680,47 @@
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="B51" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="B52" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="B53" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="B54" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="B55" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="B56" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="B57" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="B58" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="B59" t="s">
         <v>157</v>
       </c>
@@ -2719,21 +2732,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="73" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2747,7 +2760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2758,7 +2771,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2769,7 +2782,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2780,7 +2793,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -2791,7 +2804,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -2802,7 +2815,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2813,7 +2826,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -2835,7 +2848,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2846,7 +2859,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -2857,7 +2870,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2877,7 +2890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2888,7 +2901,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2899,7 +2912,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2910,7 +2923,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2921,7 +2934,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2932,7 +2945,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2943,7 +2956,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2954,7 +2967,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2962,7 +2975,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2970,7 +2983,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2978,7 +2991,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2986,7 +2999,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2994,7 +3007,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3002,7 +3015,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3013,7 +3026,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3024,7 +3037,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3035,7 +3048,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3046,7 +3059,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -3068,7 +3081,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3079,7 +3092,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3090,7 +3103,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -3101,7 +3114,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -3112,7 +3125,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3123,7 +3136,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -3131,7 +3144,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -3139,7 +3152,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3147,7 +3160,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3155,7 +3168,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -3163,7 +3176,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
admins, remove robot Krispi, chat private dialogs, fix cursor hand for FF
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
   <si>
     <t>№</t>
   </si>
@@ -854,6 +854,12 @@
   </si>
   <si>
     <t>Еще один рейтинг</t>
+  </si>
+  <si>
+    <t>Робот левел для пользователей</t>
+  </si>
+  <si>
+    <t>Чат: блокирование сообщений</t>
   </si>
 </sst>
 </file>
@@ -1381,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
@@ -2259,10 +2265,22 @@
       <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A52" s="5">
+        <v>49</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A53" s="5">
+        <v>50</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>

</xml_diff>

<commit_message>
GUI.createElement name from text to variable
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
   <si>
     <t>№</t>
   </si>
@@ -861,15 +861,21 @@
   <si>
     <t>Чат: блокирование сообщений</t>
   </si>
+  <si>
+    <t>Not Required</t>
+  </si>
+  <si>
+    <t>Not Requied</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1143,7 +1149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1175,9 +1181,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1209,6 +1216,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1384,14 +1392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1400,7 +1408,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1417,7 +1425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1434,7 +1442,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1452,7 +1460,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1470,7 +1478,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1488,7 +1496,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1506,7 +1514,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1524,7 +1532,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1542,7 +1550,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1560,7 +1568,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1578,7 +1586,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1596,7 +1604,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1614,7 +1622,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1632,7 +1640,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1650,7 +1658,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1668,7 +1676,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1686,7 +1694,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1704,7 +1712,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1722,7 +1730,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1740,7 +1748,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1758,7 +1766,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1776,7 +1784,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1794,7 +1802,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1812,7 +1820,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1830,7 +1838,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1848,7 +1856,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1866,7 +1874,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1884,7 +1892,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1902,7 +1910,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1920,21 +1928,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1952,7 +1960,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1970,7 +1978,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1988,7 +1996,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -2006,7 +2014,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -2024,7 +2032,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -2042,7 +2050,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -2060,7 +2068,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -2078,7 +2086,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -2096,7 +2104,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2114,7 +2122,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2132,7 +2140,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2150,7 +2158,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2168,7 +2176,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2186,7 +2194,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2204,7 +2212,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2222,7 +2230,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2230,10 +2238,17 @@
       <c r="B48" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2241,50 +2256,85 @@
       <c r="B49" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C50" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C51" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C52" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C53" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2302,453 +2352,236 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1">
+        <v>41969.73333333333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1">
-        <v>41969.73333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>41969.752083333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
-        <v>41969.752083333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>41969.754861111112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>41969.754861111112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2">
+        <v>41978.732638888891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2">
-        <v>41978.732638888891</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>41982.668749999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2">
-        <v>41982.667361111111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>41988.625694444447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2">
-        <v>41982.668749999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>42018.599305555559</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2">
-        <v>41982.668749999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>42018.599305555559</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2">
-        <v>41988.625694444447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>42020.539583333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="C10" s="2">
-        <v>42014.92083333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>42020.767361111109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2">
-        <v>42018.599305555559</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>42023.720138888886</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2">
-        <v>42018.599305555559</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
+        <v>42023.720138888886</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C13" s="2">
-        <v>42018.599305555559</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>42023.724999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C14" s="2">
-        <v>42018.623611111114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>42035.98333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C15" s="2">
-        <v>42018.645833333336</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>42037.756944444445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
       <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="2">
-        <v>42018.697916666664</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="2">
-        <v>42019.70208333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="2">
-        <v>42019.780555555553</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="2">
-        <v>42020.539583333331</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="2">
-        <v>42020.765972222223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="2">
-        <v>42020.767361111109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="2">
-        <v>42020.767361111109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="2">
-        <v>42023.718055555553</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="2">
-        <v>42023.720138888886</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="2">
-        <v>42023.720138888886</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="2">
-        <v>42023.724999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="2">
-        <v>42035.98333333333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="2">
-        <v>42037.756944444445</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="2">
-        <v>42038.950694444444</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="2">
-        <v>42039.758333333331</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75">
-      <c r="B31" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="2">
-        <v>42040.129861111112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" s="2">
-        <v>42040.138888888891</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="B36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="B37" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="B41" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="B42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="B43" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="B44" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="B47" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="B49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="B51" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="B52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="B53" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="B54" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="B55" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="B56" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="B57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="B58" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="B59" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2759,21 +2592,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2787,7 +2620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2798,7 +2631,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2809,7 +2642,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2820,7 +2653,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -2831,7 +2664,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -2842,7 +2675,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2853,7 +2686,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -2864,7 +2697,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -2875,7 +2708,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2886,7 +2719,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -2897,7 +2730,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2917,7 +2750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2928,7 +2761,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2939,7 +2772,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2950,7 +2783,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2961,7 +2794,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2972,7 +2805,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2983,7 +2816,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2994,7 +2827,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -3002,7 +2835,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -3010,7 +2843,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -3018,7 +2851,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -3026,7 +2859,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -3034,7 +2867,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3042,7 +2875,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3053,7 +2886,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3064,7 +2897,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3075,7 +2908,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3086,7 +2919,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3097,7 +2930,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -3108,7 +2941,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3119,7 +2952,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3130,7 +2963,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -3141,7 +2974,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -3152,7 +2985,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3163,7 +2996,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -3171,7 +3004,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -3179,7 +3012,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3187,7 +3020,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3195,7 +3028,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -3203,12 +3036,257 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
       <c r="B42" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="2">
+        <v>42018.599305555559</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="2">
+        <v>42038.950694444444</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="2">
+        <v>42039.758333333331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="2">
+        <v>41982.667361111111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="2">
+        <v>41982.668749999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="2">
+        <v>42014.92083333333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="2">
+        <v>42018.645833333336</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="2">
+        <v>42018.697916666664</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="2">
+        <v>42019.70208333333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="2">
+        <v>42019.780555555553</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="2">
+        <v>42020.765972222223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="2">
+        <v>42020.767361111109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="2">
+        <v>42023.718055555553</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="2">
+        <v>42040.129861111112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="2">
+        <v>42040.138888888891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
photo no pointer fo robo
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="171">
   <si>
     <t>№</t>
   </si>
@@ -866,6 +866,24 @@
   </si>
   <si>
     <t>Not Requied</t>
+  </si>
+  <si>
+    <t>Сделать очки  : "побед: 123" для каждой игры свой во время игры.</t>
+  </si>
+  <si>
+    <t>сделать более яркую и понятную "пригласить"</t>
+  </si>
+  <si>
+    <t>сделать надпись: свободные игроки</t>
+  </si>
+  <si>
+    <t>сделать против рейтинга знак i в кружочке при наведении вывести кард инфо игрока.</t>
+  </si>
+  <si>
+    <t>Сделать роботом еще более подстраиваемым</t>
+  </si>
+  <si>
+    <t>сделать нотификацию</t>
   </si>
 </sst>
 </file>
@@ -2353,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,89 +2518,82 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
       <c r="B19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2593,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:XFD67"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,6 +3300,70 @@
         <v>42040.138888888891</v>
       </c>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rating info, wins on PageXOGame
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="177">
   <si>
     <t>№</t>
   </si>
@@ -885,15 +885,33 @@
   <si>
     <t>сделать нотификацию</t>
   </si>
+  <si>
+    <t>виджет для крестиков надо сделать на страницы игры. Иначе при вконтактовском : оставил комментарий, человек переходит на страниц с одними только коментами, а не игрой!</t>
+  </si>
+  <si>
+    <t>выровнить числа справа у полей: рейтинг, онлайн и побед</t>
+  </si>
+  <si>
+    <t>название чатов слишком близко к полю!</t>
+  </si>
+  <si>
+    <t>в игре подчеркивать</t>
+  </si>
+  <si>
+    <t>хелп основного меню открой и посмотри, его явно надо сдвинуть нижу</t>
+  </si>
+  <si>
+    <t>showInviteDialog сделать иконки для поля и знака.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1167,7 +1185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1199,10 +1217,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1234,7 +1251,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1410,14 +1426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1426,7 +1442,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +1459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1460,7 +1476,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1478,7 +1494,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1496,7 +1512,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1514,7 +1530,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1532,7 +1548,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1550,7 +1566,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1568,7 +1584,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1586,7 +1602,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1604,7 +1620,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1622,7 +1638,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1640,7 +1656,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1658,7 +1674,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1676,7 +1692,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1694,7 +1710,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1712,7 +1728,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1730,7 +1746,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1748,7 +1764,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1766,7 +1782,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1784,7 +1800,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1802,7 +1818,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1820,7 +1836,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1838,7 +1854,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1856,7 +1872,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1874,7 +1890,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1892,7 +1908,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1910,7 +1926,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1928,7 +1944,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1946,21 +1962,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -1978,7 +1994,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -1996,7 +2012,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -2014,7 +2030,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -2032,7 +2048,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -2050,7 +2066,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -2068,7 +2084,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -2086,7 +2102,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -2104,7 +2120,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -2122,7 +2138,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2140,7 +2156,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2158,7 +2174,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2176,7 +2192,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2194,7 +2210,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2212,7 +2228,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2230,7 +2246,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2248,7 +2264,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2266,7 +2282,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2284,7 +2300,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="A50" s="5">
         <v>47</v>
       </c>
@@ -2301,7 +2317,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" s="5">
         <v>48</v>
       </c>
@@ -2318,7 +2334,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="5">
         <v>49</v>
       </c>
@@ -2335,7 +2351,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="A53" s="5">
         <v>50</v>
       </c>
@@ -2352,7 +2368,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
@@ -2370,21 +2386,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -2392,7 +2408,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -2400,7 +2416,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -2408,7 +2424,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -2416,7 +2432,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -2424,7 +2440,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2435,7 +2451,7 @@
         <v>41988.625694444447</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -2443,7 +2459,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -2451,7 +2467,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>88</v>
       </c>
@@ -2459,7 +2475,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>92</v>
       </c>
@@ -2467,7 +2483,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>95</v>
       </c>
@@ -2475,7 +2491,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>96</v>
       </c>
@@ -2483,7 +2499,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" t="s">
         <v>97</v>
       </c>
@@ -2491,7 +2507,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>99</v>
       </c>
@@ -2499,7 +2515,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -2510,7 +2526,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -2518,17 +2534,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="B17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="B18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -2536,64 +2552,94 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="B20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="B21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="B22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="B23" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="B24" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="B25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="B26" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="B27" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="B28" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="B29" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="B30" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2603,21 +2649,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A75" sqref="A75:B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="73" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2631,7 +2677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2642,7 +2688,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2653,7 +2699,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2664,7 +2710,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -2675,7 +2721,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -2686,7 +2732,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2697,7 +2743,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -2708,7 +2754,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -2719,7 +2765,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2730,7 +2776,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -2741,7 +2787,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2761,7 +2807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2772,7 +2818,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2783,7 +2829,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2840,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2805,7 +2851,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2816,7 +2862,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2827,7 +2873,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2838,7 +2884,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2846,7 +2892,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2854,7 +2900,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2862,7 +2908,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2870,7 +2916,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2878,7 +2924,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2886,7 +2932,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2897,7 +2943,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2908,7 +2954,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2919,7 +2965,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2930,7 +2976,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2941,7 +2987,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2952,7 +2998,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2963,7 +3009,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -2974,7 +3020,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -2985,7 +3031,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -2996,7 +3042,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3007,7 +3053,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -3015,7 +3061,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -3023,7 +3069,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3031,7 +3077,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3039,7 +3085,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -3047,7 +3093,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -3055,7 +3101,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -3066,7 +3112,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -3077,7 +3123,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -3088,7 +3134,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3096,7 +3142,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -3104,7 +3150,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -3112,7 +3158,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -3120,7 +3166,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -3128,7 +3174,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -3136,7 +3182,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -3144,7 +3190,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -3152,7 +3198,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -3160,7 +3206,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -3171,7 +3217,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>124</v>
       </c>
@@ -3182,7 +3228,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -3193,7 +3239,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -3201,7 +3247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3212,7 +3258,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -3223,7 +3269,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>164</v>
       </c>
@@ -3234,7 +3280,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -3245,7 +3291,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -3256,7 +3302,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -3267,7 +3313,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -3278,7 +3324,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15.75">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -3289,7 +3335,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -3300,7 +3346,7 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -3308,7 +3354,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -3316,7 +3362,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>163</v>
       </c>
@@ -3324,7 +3370,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -3332,7 +3378,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>26</v>
       </c>
@@ -3340,7 +3386,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>26</v>
       </c>
@@ -3348,7 +3394,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -3356,7 +3402,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
realize notifier, some fixes, one host - many services and so on
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="181">
   <si>
     <t>№</t>
   </si>
@@ -908,6 +908,12 @@
   </si>
   <si>
     <t>сделать новые собщения(если не читал)</t>
+  </si>
+  <si>
+    <t>Чат, приватный.</t>
+  </si>
+  <si>
+    <t>Нотифиер.</t>
   </si>
 </sst>
 </file>
@@ -1435,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2377,8 +2383,29 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="A54" s="5">
+        <v>51</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>52</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2397,7 +2424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some...after many days man :)
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="205">
   <si>
     <t>№</t>
   </si>
@@ -915,15 +915,87 @@
   <si>
     <t>Нотифиер.</t>
   </si>
+  <si>
+    <t>Сделать выбор знака более удобным: случайного например сейчас просто нет!</t>
+  </si>
+  <si>
+    <t>Сделать поле 19 на 19!, сделать однако три режима 3х3,15х15,19х19</t>
+  </si>
+  <si>
+    <t>Сизый Пепел говорит, хорошо бы пришли ребята посильней.</t>
+  </si>
+  <si>
+    <t>поискать сообщетсва профессиональных игроков</t>
+  </si>
+  <si>
+    <t>сделать версию не через ВК</t>
+  </si>
+  <si>
+    <t>сделать настройки: убрать 3 на 3.</t>
+  </si>
+  <si>
+    <t>узнать про чемпиона Илья Муратова России в гомоку</t>
+  </si>
+  <si>
+    <t>комменты фоток постов, т.е. на стене есть мессдж, а вот на самой фотке нет.</t>
+  </si>
+  <si>
+    <t>Сделать кнопку,Сменить знак!</t>
+  </si>
+  <si>
+    <t>http://logic-games.spb.ru/gomoku/debut/</t>
+  </si>
+  <si>
+    <t>прочесть https://vk.com/photo-23971927_219679564</t>
+  </si>
+  <si>
+    <t>доработать хелп</t>
+  </si>
+  <si>
+    <t>визард!</t>
+  </si>
+  <si>
+    <t>послдний ход лучше выделить</t>
+  </si>
+  <si>
+    <t>блиц</t>
+  </si>
+  <si>
+    <t>таймер</t>
+  </si>
+  <si>
+    <t>подсветка опасных ходов, она же подсказка об обороне, сообщить потом Электро Току</t>
+  </si>
+  <si>
+    <t>рейтинг ЭЛО, сообщить электро Ток и Сизый пепел</t>
+  </si>
+  <si>
+    <t>Сизый Пепел предлагает Блиц режим, сообщить ему об этом потом!)</t>
+  </si>
+  <si>
+    <t>пять в рядо \ гомоку или рендзю?</t>
+  </si>
+  <si>
+    <t>разряды для рейтинга</t>
+  </si>
+  <si>
+    <t>бордюр фоток под новый фон</t>
+  </si>
+  <si>
+    <t>иконку игы под новый фон</t>
+  </si>
+  <si>
+    <t>картинку в группе под новый фон</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1197,7 +1269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1229,10 +1301,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1264,7 +1335,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1440,14 +1510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="32" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1456,7 +1526,7 @@
     <col min="6" max="16384" width="32" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1490,7 +1560,7 @@
         <v>41967.652777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <f>A2+1</f>
         <v>2</v>
@@ -1508,7 +1578,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -1526,7 +1596,7 @@
         <v>41968.9375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1544,7 +1614,7 @@
         <v>41969.786805555559</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1562,7 +1632,7 @@
         <v>41975.571527777778</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1580,7 +1650,7 @@
         <v>41975.586805555555</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1598,7 +1668,7 @@
         <v>41978.646527777775</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1616,7 +1686,7 @@
         <v>41978.736805555556</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1634,7 +1704,7 @@
         <v>41981.65347222222</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="13">
         <f>A10+1</f>
         <v>10</v>
@@ -1652,7 +1722,7 @@
         <v>41982.694444444445</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="15">
         <f t="shared" ref="A12:A29" si="1">A11+1</f>
         <v>11</v>
@@ -1670,7 +1740,7 @@
         <v>41982.727083333331</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1688,7 +1758,7 @@
         <v>41983.770833333336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1706,7 +1776,7 @@
         <v>41985.643750000003</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1724,7 +1794,7 @@
         <v>41985.713888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1742,7 +1812,7 @@
         <v>41987.615972222222</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1760,7 +1830,7 @@
         <v>41987.707638888889</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1778,7 +1848,7 @@
         <v>41987.765277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -1796,7 +1866,7 @@
         <v>41989.681944444441</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="13">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1814,7 +1884,7 @@
         <v>41988.74722222222</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="15">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1832,7 +1902,7 @@
         <v>41989.708333333336</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1850,7 +1920,7 @@
         <v>41996.762499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1868,7 +1938,7 @@
         <v>41996.859027777777</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1886,7 +1956,7 @@
         <v>41998.57708333333</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1904,7 +1974,7 @@
         <v>41999.48333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="13">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1922,7 +1992,7 @@
         <v>41999.656944444447</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="15">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1940,7 +2010,7 @@
         <v>42002.667361111111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1958,7 +2028,7 @@
         <v>42006.01666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="36">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1976,21 +2046,21 @@
         <v>42006.890277777777</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="36"/>
       <c r="B30" s="30"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="34"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="37"/>
       <c r="B31" s="31"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="35"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="15">
         <f>A29+1</f>
         <v>29</v>
@@ -2008,7 +2078,7 @@
         <v>42010.81527777778</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <f t="shared" ref="A33:A49" si="2">A32+1</f>
         <v>30</v>
@@ -2026,7 +2096,7 @@
         <v>42011.962500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -2044,7 +2114,7 @@
         <v>42013.111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
       <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -2062,7 +2132,7 @@
         <v>42013.80972222222</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -2080,7 +2150,7 @@
         <v>42014.041666666664</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -2098,7 +2168,7 @@
         <v>42014.952777777777</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -2116,7 +2186,7 @@
         <v>42015.051388888889</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -2134,7 +2204,7 @@
         <v>42017.60833333333</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -2152,7 +2222,7 @@
         <v>42017.772222222222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="10">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2170,7 +2240,7 @@
         <v>42018.723611111112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
       <c r="A42" s="13">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2188,7 +2258,7 @@
         <v>42019.777083333334</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="15">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2206,7 +2276,7 @@
         <v>42020.709722222222</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2224,7 +2294,7 @@
         <v>42020.720138888886</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2242,7 +2312,7 @@
         <v>42020.774305555555</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" s="13">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2260,7 +2330,7 @@
         <v>42023.731944444444</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2278,7 +2348,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2296,7 +2366,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2314,7 +2384,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1">
       <c r="A50" s="5">
         <v>47</v>
       </c>
@@ -2331,7 +2401,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" s="5">
         <v>48</v>
       </c>
@@ -2348,7 +2418,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="5">
         <v>49</v>
       </c>
@@ -2365,7 +2435,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="A53" s="5">
         <v>50</v>
       </c>
@@ -2382,7 +2452,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="A54" s="5">
         <v>51</v>
       </c>
@@ -2399,7 +2469,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="15.75" customHeight="1">
       <c r="A55" s="5">
         <v>52</v>
       </c>
@@ -2421,29 +2491,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1">
-        <v>41969.73333333333</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -2451,7 +2513,7 @@
         <v>41969.752083333333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -2459,7 +2521,7 @@
         <v>41969.754861111112</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -2467,7 +2529,7 @@
         <v>41978.732638888891</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -2475,18 +2537,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2">
-        <v>41988.625694444447</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -2494,7 +2545,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -2502,7 +2553,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>88</v>
       </c>
@@ -2510,7 +2561,7 @@
         <v>42020.539583333331</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -2521,7 +2572,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>95</v>
       </c>
@@ -2529,7 +2580,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>96</v>
       </c>
@@ -2537,7 +2588,7 @@
         <v>42023.720138888886</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" t="s">
         <v>97</v>
       </c>
@@ -2545,7 +2596,7 @@
         <v>42023.724999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>99</v>
       </c>
@@ -2553,7 +2604,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -2561,17 +2612,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="B17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -2579,37 +2630,37 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="B19" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="B20" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="B21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="B22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="B23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="B24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -2617,12 +2668,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="B27" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>176</v>
       </c>
@@ -2630,7 +2681,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>176</v>
       </c>
@@ -2638,17 +2689,17 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="B30" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>176</v>
       </c>
@@ -2656,22 +2707,147 @@
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="B33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="B34" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>176</v>
       </c>
       <c r="B35" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="B37" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="B38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="B39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="B41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="B43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2681,21 +2857,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:B79"/>
+      <selection activeCell="A81" sqref="A81:C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="73" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -2709,7 +2885,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -2720,7 +2896,7 @@
         <v>41969.676388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -2731,7 +2907,7 @@
         <v>41969.681944444441</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -2742,7 +2918,7 @@
         <v>41969.696527777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -2753,7 +2929,7 @@
         <v>41969.740972222222</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -2764,7 +2940,7 @@
         <v>41969.743055555555</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2775,7 +2951,7 @@
         <v>41973.410416666666</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -2786,7 +2962,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -2797,7 +2973,7 @@
         <v>41974.5625</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2808,7 +2984,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -2819,7 +2995,7 @@
         <v>41975.691666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2839,7 +3015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2850,7 +3026,7 @@
         <v>41974.617361111108</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2861,7 +3037,7 @@
         <v>41975.678472222222</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2872,7 +3048,7 @@
         <v>42018.645138888889</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2883,7 +3059,7 @@
         <v>42035.98333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2894,7 +3070,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2905,7 +3081,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2916,7 +3092,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2924,7 +3100,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2932,7 +3108,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2940,7 +3116,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2948,7 +3124,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2956,7 +3132,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2964,7 +3140,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2975,7 +3151,7 @@
         <v>41969.73333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2986,7 +3162,7 @@
         <v>42013.963194444441</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2997,7 +3173,7 @@
         <v>42018.640972222223</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3008,7 +3184,7 @@
         <v>42019.782638888886</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3019,7 +3195,7 @@
         <v>42020.76666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -3030,7 +3206,7 @@
         <v>42029.820833333331</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3041,7 +3217,7 @@
         <v>42038.629861111112</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3052,7 +3228,7 @@
         <v>42038.938888888886</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -3063,7 +3239,7 @@
         <v>42040.081944444442</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -3074,7 +3250,7 @@
         <v>42040.088194444441</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3085,7 +3261,7 @@
         <v>42040.140277777777</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -3093,7 +3269,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -3101,7 +3277,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3109,7 +3285,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3117,7 +3293,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -3125,7 +3301,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -3133,7 +3309,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -3144,7 +3320,7 @@
         <v>42018.599305555559</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -3155,7 +3331,7 @@
         <v>42038.950694444444</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -3166,7 +3342,7 @@
         <v>42039.758333333331</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3174,7 +3350,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -3182,7 +3358,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -3190,7 +3366,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -3198,7 +3374,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -3206,7 +3382,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -3214,7 +3390,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -3222,7 +3398,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -3230,7 +3406,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -3238,7 +3414,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -3249,7 +3425,7 @@
         <v>41982.667361111111</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>124</v>
       </c>
@@ -3260,7 +3436,7 @@
         <v>41982.668749999997</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -3271,7 +3447,7 @@
         <v>42014.92083333333</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -3279,7 +3455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3290,7 +3466,7 @@
         <v>42018.645833333336</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -3301,7 +3477,7 @@
         <v>42018.697916666664</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>164</v>
       </c>
@@ -3312,7 +3488,7 @@
         <v>42019.70208333333</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -3323,7 +3499,7 @@
         <v>42019.780555555553</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -3334,7 +3510,7 @@
         <v>42020.765972222223</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -3345,7 +3521,7 @@
         <v>42020.767361111109</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -3356,7 +3532,7 @@
         <v>42023.718055555553</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15.75">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -3367,7 +3543,7 @@
         <v>42040.129861111112</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -3378,7 +3554,7 @@
         <v>42040.138888888891</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -3386,7 +3562,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -3394,7 +3570,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>163</v>
       </c>
@@ -3402,7 +3578,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -3410,7 +3586,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>26</v>
       </c>
@@ -3418,7 +3594,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>26</v>
       </c>
@@ -3426,7 +3602,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -3434,7 +3610,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -3442,7 +3618,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -3453,7 +3629,7 @@
         <v>42037.756944444445</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -3461,7 +3637,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -3469,12 +3645,34 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>26</v>
       </c>
       <c r="B79" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C80" s="2">
+        <v>41988.625694444447</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="1">
+        <v>41969.73333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>